<commit_message>
#update get all data in api settle to export
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-Detail Template.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-Detail Template.xlsx
@@ -18,285 +18,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Thai Phuong</author>
-  </authors>
-  <commentList>
-    <comment ref="Y3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Hiện Thông tin Advance no trên dòng tổng group theo job</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- group 1 Tổng advance Amount Tren Settlement
-- Group 2 Tổng advance Amount Theo Lô hàng và advance
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-- group 1 Tổng balance Tren Settlement
-- Group 2 Tổng balance Theo Lô hàng và advance
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Hiện Thông tin Payment Method Settlement trên dòng group Settlement</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AD3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Hiện Thông tin Due Date Settlement trên dòng group Settlement</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AE3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Hiện Thông tin bank Account No Settlement trên dòng group Settlement</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AF3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Hiện Thông tin bank Account Name Settlement trên dòng group Settlement</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AG3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Hiện Thông tin bank Name Settlement trên dòng group Settlement</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Total Settlement Amount
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Total Adavance amount</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Thai Phuong:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Total Advance - Total Settlement</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
@@ -570,7 +291,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ \ hh:mm:ss\ AM/PM"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -590,19 +311,6 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -703,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -713,7 +421,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -753,7 +460,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -774,7 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -785,18 +490,20 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="37" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="37" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="37" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1077,29 +784,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="12.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.08984375" style="4" customWidth="1"/>
     <col min="4" max="4" width="16" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="24.26953125" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="13.1796875" style="12" customWidth="1"/>
-    <col min="14" max="14" width="17.6328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" style="12" customWidth="1"/>
-    <col min="16" max="16" width="13.1796875" style="18" customWidth="1"/>
-    <col min="17" max="18" width="13.1796875" style="12" customWidth="1"/>
-    <col min="19" max="19" width="39.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="24" width="13.1796875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="23.81640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="7.36328125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" style="11" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="11" customWidth="1"/>
+    <col min="14" max="14" width="17.6328125" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1796875" style="11" customWidth="1"/>
+    <col min="16" max="16" width="13.1796875" style="17" customWidth="1"/>
+    <col min="17" max="18" width="13.1796875" style="11" customWidth="1"/>
+    <col min="19" max="19" width="39.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="24" width="13.1796875" style="11" customWidth="1"/>
     <col min="25" max="25" width="11.7265625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="16.81640625" style="8" customWidth="1"/>
-    <col min="27" max="27" width="14" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.81640625" style="7" customWidth="1"/>
+    <col min="27" max="27" width="14" style="10" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="22.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="16.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="17.54296875" style="4" bestFit="1" customWidth="1"/>
@@ -1119,26 +833,26 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="9"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="8"/>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
@@ -1154,366 +868,366 @@
       <c r="AN1" s="2"/>
     </row>
     <row r="2" spans="1:40" customFormat="1">
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="10"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="9"/>
     </row>
     <row r="3" spans="1:40" s="3" customFormat="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="23" t="s">
+      <c r="P3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="U3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X3" s="21" t="s">
+      <c r="X3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Y3" s="21" t="s">
+      <c r="Y3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="Z3" s="24" t="s">
+      <c r="Z3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="23" t="s">
+      <c r="AA3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="AB3" s="21" t="s">
+      <c r="AB3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AC3" s="21" t="s">
+      <c r="AC3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AD3" s="21" t="s">
+      <c r="AD3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AE3" s="21" t="s">
+      <c r="AE3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AF3" s="21" t="s">
+      <c r="AF3" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AG3" s="21" t="s">
+      <c r="AG3" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:40" customFormat="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="55" t="s">
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="O4" s="39"/>
-      <c r="P4" s="58" t="s">
+      <c r="O4" s="37"/>
+      <c r="P4" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="Q4" s="61" t="s">
+      <c r="Q4" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R4" s="61" t="s">
+      <c r="R4" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="64" t="s">
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="33"/>
+      <c r="Z4" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="AA4" s="66" t="s">
+      <c r="AA4" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="AB4" s="35" t="s">
+      <c r="AB4" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="AC4" s="37" t="s">
+      <c r="AC4" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="AD4" s="36" t="s">
+      <c r="AD4" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="37" t="s">
+      <c r="AE4" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="AF4" s="37" t="s">
+      <c r="AF4" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="AG4" s="38" t="s">
+      <c r="AG4" s="36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:40" s="46" customFormat="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42" t="s">
+    <row r="5" spans="1:40" s="43" customFormat="1">
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="44" t="s">
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="O5" s="43"/>
-      <c r="P5" s="56" t="s">
+      <c r="O5" s="41"/>
+      <c r="P5" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="Q5" s="59" t="s">
+      <c r="Q5" s="55" t="s">
         <v>81</v>
       </c>
       <c r="R5" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="43"/>
-      <c r="T5" s="43"/>
-      <c r="U5" s="43"/>
-      <c r="V5" s="43"/>
-      <c r="W5" s="43"/>
-      <c r="X5" s="43"/>
-      <c r="Y5" s="42" t="s">
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="Z5" s="63" t="s">
+      <c r="Z5" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="AA5" s="65" t="s">
+      <c r="AA5" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="41"/>
-      <c r="AE5" s="41"/>
-      <c r="AF5" s="41"/>
-      <c r="AG5" s="45"/>
+      <c r="AB5" s="40"/>
+      <c r="AC5" s="39"/>
+      <c r="AD5" s="39"/>
+      <c r="AE5" s="39"/>
+      <c r="AF5" s="39"/>
+      <c r="AG5" s="42"/>
     </row>
     <row r="6" spans="1:40" customFormat="1">
-      <c r="A6" s="32"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="L6" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="26" t="s">
+      <c r="M6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="O6" s="54" t="s">
+      <c r="O6" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="P6" s="57" t="s">
+      <c r="P6" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="60" t="s">
+      <c r="Q6" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="R6" s="62" t="s">
+      <c r="R6" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="S6" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="54" t="s">
+      <c r="T6" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="U6" s="54" t="s">
+      <c r="U6" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="V6" s="54" t="s">
+      <c r="V6" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="W6" s="54" t="s">
+      <c r="W6" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="X6" s="54" t="s">
+      <c r="X6" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="Y6" s="54"/>
-      <c r="Z6" s="28"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="30"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="47"/>
+      <c r="Y6" s="51"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="44"/>
     </row>
     <row r="7" spans="1:40">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
-      <c r="U7" s="49"/>
-      <c r="V7" s="49"/>
-      <c r="W7" s="49"/>
-      <c r="X7" s="49"/>
-      <c r="Y7" s="48"/>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="53"/>
-      <c r="AB7" s="48"/>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="48"/>
-      <c r="AE7" s="48"/>
-      <c r="AF7" s="48"/>
-      <c r="AG7" s="48"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="46"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="46"/>
+      <c r="R7" s="46"/>
+      <c r="S7" s="46"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="46"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="49"/>
+      <c r="AA7" s="50"/>
+      <c r="AB7" s="45"/>
+      <c r="AC7" s="45"/>
+      <c r="AD7" s="45"/>
+      <c r="AE7" s="45"/>
+      <c r="AF7" s="45"/>
+      <c r="AG7" s="45"/>
     </row>
     <row r="10" spans="1:40">
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="65" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1521,7 +1235,7 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="65" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1529,13 +1243,12 @@
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="65" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#update format number and date
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-Detail Template.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/SettlePayment/Settlement-Detail Template.xlsx
@@ -499,11 +499,11 @@
     <xf numFmtId="37" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="37" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="37" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="39" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="39" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -787,9 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -1009,7 +1007,7 @@
       <c r="K4" s="37"/>
       <c r="L4" s="37"/>
       <c r="M4" s="37"/>
-      <c r="N4" s="58" t="s">
+      <c r="N4" s="53" t="s">
         <v>73</v>
       </c>
       <c r="O4" s="37"/>
@@ -1029,10 +1027,10 @@
       <c r="W4" s="37"/>
       <c r="X4" s="37"/>
       <c r="Y4" s="33"/>
-      <c r="Z4" s="63" t="s">
+      <c r="Z4" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="AA4" s="63" t="s">
+      <c r="AA4" s="61" t="s">
         <v>85</v>
       </c>
       <c r="AB4" s="33" t="s">
@@ -1076,7 +1074,7 @@
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
       <c r="M5" s="41"/>
-      <c r="N5" s="61" t="s">
+      <c r="N5" s="65" t="s">
         <v>72</v>
       </c>
       <c r="O5" s="41"/>
@@ -1098,10 +1096,10 @@
       <c r="Y5" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="Z5" s="64" t="s">
+      <c r="Z5" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="AA5" s="64" t="s">
+      <c r="AA5" s="62" t="s">
         <v>86</v>
       </c>
       <c r="AB5" s="40"/>
@@ -1133,19 +1131,19 @@
       <c r="I6" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="64" t="s">
         <v>48</v>
       </c>
       <c r="K6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="L6" s="62" t="s">
+      <c r="L6" s="64" t="s">
         <v>46</v>
       </c>
       <c r="M6" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="62" t="s">
+      <c r="N6" s="64" t="s">
         <v>50</v>
       </c>
       <c r="O6" s="51" t="s">
@@ -1227,7 +1225,7 @@
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="63" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1235,7 +1233,7 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="63" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1243,7 +1241,7 @@
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="63" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>